<commit_message>
Updated the config files, removed unneeded ones, added some new ones
</commit_message>
<xml_diff>
--- a/config/only valve and only pumonary extended Phentermine cardio adr.xlsx
+++ b/config/only valve and only pumonary extended Phentermine cardio adr.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/boris/temp/paper configs/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{36B8E305-668C-6242-A6E9-9A96258D9681}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17400" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name=" pulmonary (3)" sheetId="5" r:id="rId1"/>
-    <sheet name="valave " sheetId="4" r:id="rId2"/>
+    <sheet name=" pulmonary" sheetId="5" r:id="rId1"/>
+    <sheet name="valve " sheetId="4" r:id="rId2"/>
     <sheet name="cardio non valve and pulmonary" sheetId="1" r:id="rId3"/>
-    <sheet name="valave and pulmonary" sheetId="2" r:id="rId4"/>
+    <sheet name="valve and pulmonary" sheetId="2" r:id="rId4"/>
     <sheet name="cardio total" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -1030,12 +1036,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -1394,27 +1400,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B71"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:B71"/>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.19921875" customWidth="1"/>
-    <col min="2" max="2" width="36.19921875" customWidth="1"/>
+    <col min="1" max="1" width="23.1640625" customWidth="1"/>
+    <col min="2" max="2" width="36.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -1422,7 +1428,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -1430,7 +1436,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1438,7 +1444,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -1446,7 +1452,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
@@ -1454,7 +1460,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -1462,7 +1468,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -1470,7 +1476,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -1478,7 +1484,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
@@ -1486,7 +1492,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -1494,7 +1500,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -1502,7 +1508,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
@@ -1510,7 +1516,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -1518,189 +1524,181 @@
         <v>284</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B14" s="7"/>
     </row>
-    <row r="15" spans="1:2" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" s="7"/>
     </row>
-    <row r="16" spans="1:2" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B16" s="7"/>
     </row>
-    <row r="17" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B17" s="8"/>
     </row>
-    <row r="18" spans="2:2" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B18" s="7"/>
     </row>
-    <row r="19" spans="2:2" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B19" s="7"/>
     </row>
-    <row r="20" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B20" s="8"/>
     </row>
-    <row r="21" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="8"/>
     </row>
-    <row r="22" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B22" s="8"/>
     </row>
-    <row r="23" spans="2:2" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B23" s="7"/>
     </row>
-    <row r="24" spans="2:2" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B24" s="7"/>
     </row>
-    <row r="25" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B25" s="8"/>
     </row>
-    <row r="26" spans="2:2" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B26" s="7"/>
     </row>
-    <row r="27" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B27" s="8"/>
     </row>
-    <row r="28" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B28" s="8"/>
     </row>
-    <row r="29" spans="2:2" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B29" s="7"/>
     </row>
-    <row r="30" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B30" s="8"/>
     </row>
-    <row r="31" spans="2:2" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B31" s="7"/>
     </row>
-    <row r="32" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B32" s="8"/>
     </row>
-    <row r="33" spans="2:2" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B33" s="7"/>
     </row>
-    <row r="34" spans="2:2" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B34" s="7"/>
     </row>
-    <row r="35" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B35" s="8"/>
     </row>
-    <row r="36" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B36" s="8"/>
     </row>
-    <row r="37" spans="2:2" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B37" s="7"/>
     </row>
-    <row r="38" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B38" s="8"/>
     </row>
-    <row r="39" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B39" s="8"/>
     </row>
-    <row r="40" spans="2:2" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B40" s="7"/>
     </row>
-    <row r="41" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B41" s="8"/>
     </row>
-    <row r="42" spans="2:2" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B42" s="7"/>
     </row>
-    <row r="43" spans="2:2" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B43" s="7"/>
     </row>
-    <row r="44" spans="2:2" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B44" s="7"/>
     </row>
-    <row r="45" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B45" s="8"/>
     </row>
-    <row r="46" spans="2:2" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B46" s="7"/>
     </row>
-    <row r="47" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B47" s="8"/>
     </row>
-    <row r="48" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B48" s="8"/>
     </row>
-    <row r="49" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B49" s="8"/>
     </row>
-    <row r="50" spans="2:2" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B50" s="7"/>
     </row>
-    <row r="51" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B51" s="8"/>
     </row>
-    <row r="52" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B52" s="8"/>
     </row>
-    <row r="53" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B53" s="8"/>
     </row>
-    <row r="54" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B54" s="8"/>
     </row>
-    <row r="55" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B55" s="8"/>
     </row>
-    <row r="56" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B56" s="8"/>
     </row>
-    <row r="57" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B57" s="2"/>
     </row>
-    <row r="58" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B58" s="2"/>
     </row>
-    <row r="59" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B59" s="2"/>
     </row>
-    <row r="60" spans="2:2" ht="14.25" x14ac:dyDescent="0.2"/>
-    <row r="61" spans="2:2" ht="14.25" x14ac:dyDescent="0.2"/>
-    <row r="62" spans="2:2" ht="14.25" x14ac:dyDescent="0.2"/>
-    <row r="63" spans="2:2" ht="14.25" x14ac:dyDescent="0.2"/>
-    <row r="64" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B64" s="2"/>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B65" s="3"/>
     </row>
-    <row r="66" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B66" s="2"/>
     </row>
-    <row r="67" spans="2:2" ht="14.25" x14ac:dyDescent="0.2"/>
-    <row r="68" spans="2:2" ht="14.25" x14ac:dyDescent="0.2"/>
-    <row r="69" spans="2:2" ht="14.25" x14ac:dyDescent="0.2"/>
-    <row r="70" spans="2:2" ht="14.25" x14ac:dyDescent="0.2"/>
-    <row r="71" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B71" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="http://bioportal.bioontology.org/ontologies/ICD10?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FICD10%2FI05.9"/>
-    <hyperlink ref="B8" r:id="rId2" display="http://bioportal.bioontology.org/ontologies/CRISP?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FCSP%2F1393-3777"/>
-    <hyperlink ref="B10" r:id="rId3" display="http://bioportal.bioontology.org/ontologies/SNOMEDCT?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FSNOMEDCT%2F194732001"/>
+    <hyperlink ref="B2" r:id="rId1" display="http://bioportal.bioontology.org/ontologies/ICD10?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FICD10%2FI05.9" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B8" r:id="rId2" display="http://bioportal.bioontology.org/ontologies/CRISP?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FCSP%2F1393-3777" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B10" r:id="rId3" display="http://bioportal.bioontology.org/ontologies/SNOMEDCT?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FSNOMEDCT%2F194732001" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
+    <sheetView rightToLeft="1" topLeftCell="A40" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.19921875" customWidth="1"/>
-    <col min="2" max="2" width="36.19921875" customWidth="1"/>
+    <col min="1" max="1" width="23.1640625" customWidth="1"/>
+    <col min="2" max="2" width="36.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -1708,7 +1706,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -1716,7 +1714,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1724,7 +1722,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -1732,7 +1730,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
@@ -1740,7 +1738,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -1748,7 +1746,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -1756,7 +1754,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -1764,7 +1762,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
@@ -1772,7 +1770,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -1780,7 +1778,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -1788,7 +1786,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
@@ -1796,7 +1794,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -1804,264 +1802,264 @@
         <v>293</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B14" s="8" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B15" s="7" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B16" s="8" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B17" s="8" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B18" s="7" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B19" s="8" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B20" s="7" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="8" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="22" spans="2:2" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B22" s="7" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="23" spans="2:2" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B23" s="7" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="24" spans="2:2" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B24" s="8" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="25" spans="2:2" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B25" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="2:2" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B26" s="7" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="27" spans="2:2" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B27" s="8" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="28" spans="2:2" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B28" s="8" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="29" spans="2:2" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B29" s="7" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="30" spans="2:2" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B30" s="8" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="31" spans="2:2" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B31" s="7" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="32" spans="2:2" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B32" s="7" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="33" spans="2:2" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B33" s="7" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="34" spans="2:2" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B34" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="2:2" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B35" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="2:2" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B36" s="8" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="37" spans="2:2" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B37" s="8" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="38" spans="2:2" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B38" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="2:2" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B39" s="7" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="40" spans="2:2" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B40" s="8" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="41" spans="2:2" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B41" s="8" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="42" spans="2:2" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B42" s="8" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="43" spans="2:2" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B43" s="8" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="44" spans="2:2" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B44" s="8" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="45" spans="2:2" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B45" s="8" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B46" s="2" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B47" s="2" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B53" s="2" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B54" s="3" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B55" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B60" s="2" t="s">
         <v>333</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B15" r:id="rId1" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10026985"/>
+    <hyperlink ref="B15" r:id="rId1" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10026985" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B252"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.09765625" customWidth="1"/>
-    <col min="2" max="2" width="45.8984375" customWidth="1"/>
+    <col min="1" max="1" width="23.1640625" customWidth="1"/>
+    <col min="2" max="2" width="45.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -2069,7 +2067,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -2077,7 +2075,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -2085,7 +2083,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -2093,7 +2091,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
@@ -2101,7 +2099,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -2109,7 +2107,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -2117,7 +2115,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -2125,7 +2123,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
@@ -2133,7 +2131,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -2141,7 +2139,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -2149,7 +2147,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
@@ -2157,7 +2155,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -2165,1219 +2163,1219 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B23" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B24" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B26" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B27" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B28" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B29" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B30" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B31" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B32" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B36" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B37" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="38" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B38" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B39" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B40" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B41" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B42" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B43" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="44" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B44" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="45" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B45" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="46" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B46" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B47" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="48" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B48" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="49" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B49" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="50" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B50" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="51" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B51" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="52" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B52" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="53" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B53" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="54" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B54" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="55" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B55" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="56" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B56" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="57" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B57" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="58" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B58" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="59" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B59" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="60" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B60" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="61" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B61" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="62" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B62" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="63" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B63" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="64" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B64" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="65" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B65" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="66" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B66" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="67" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="68" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B68" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="69" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B69" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="70" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B70" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="71" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B71" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="72" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B72" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="73" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B73" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="74" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B74" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="75" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B75" s="6" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="76" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="77" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B77" s="4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="78" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B78" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="79" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B79" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="80" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B80" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="81" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B81" s="5" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="82" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B82" s="5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="83" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B83" s="5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="84" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B84" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="85" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B85" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="86" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B86" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="87" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B87" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="88" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B88" s="5" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="89" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B89" s="4" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="90" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B90" s="5" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="91" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B91" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="92" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B92" s="4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="93" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B93" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="94" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B94" s="5" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="95" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B95" s="4" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="96" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B96" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B97" s="4" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="98" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B98" s="5" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="99" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B99" s="5" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="100" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B100" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="101" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B101" s="4" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="102" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B102" s="3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="103" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B103" s="4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="104" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B104" s="4" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="105" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B105" s="5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="106" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B106" s="4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="107" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B107" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="108" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B108" s="5" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="109" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B109" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B110" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B111" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="112" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B112" s="4" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="113" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B113" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="114" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B114" s="4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="115" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B115" s="3" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="116" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B116" s="3" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="117" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B117" s="4" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="118" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B118" s="4" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="119" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B119" s="5" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="120" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B120" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B121" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B122" s="4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="123" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B123" s="4" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="124" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B124" s="5" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="125" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B125" s="5" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="126" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B126" s="5" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="127" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B127" s="5" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="128" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B128" s="4" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="129" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B129" s="5" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="130" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B130" s="4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="131" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B131" s="4" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="132" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B132" s="3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="133" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="133" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B133" s="3" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="134" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="134" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B134" s="3" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="135" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B135" s="3" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="136" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B136" s="3" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="137" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B137" s="3" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="138" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B138" s="3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="139" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B139" s="3" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="140" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B140" s="3" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="141" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B141" s="3" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="142" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B142" s="3" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="143" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B143" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="144" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="144" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B144" s="3" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="145" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="145" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B145" s="4" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="146" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B146" s="4" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="147" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B147" s="5" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="148" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B148" s="5" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="149" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B149" s="4" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="150" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B150" s="2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="151" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B151" s="3" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="152" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B152" s="3" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="153" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B153" s="3" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="154" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B154" s="3" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="155" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="155" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B155" s="3" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="156" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="156" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B156" s="3" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="157" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="157" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B157" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="158" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B158" s="3" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="159" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="159" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B159" s="3" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="160" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="160" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B160" s="3" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="161" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="161" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B161" s="3" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="162" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="162" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B162" s="3" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="163" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="163" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B163" s="3" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="164" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="164" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B164" s="3" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="165" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="165" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B165" s="3" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="166" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="166" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B166" s="3" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="167" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="167" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B167" s="3" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="168" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="168" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B168" s="3" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="169" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="169" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B169" s="3" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="170" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="170" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B170" s="3" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="171" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="171" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B171" s="3" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="172" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="172" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B172" s="3" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="173" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="173" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B173" s="3" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="174" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="174" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B174" s="3" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="175" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="175" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B175" s="3" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="176" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="176" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B176" s="3" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="177" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="177" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B177" s="3" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="178" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="178" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B178" s="3" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="179" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="179" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B179" s="3" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="180" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="180" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B180" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="181" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="181" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B181" s="3" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="182" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="182" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B182" s="3" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="183" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="183" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B183" s="3" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="184" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="184" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B184" s="3" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="185" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="185" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B185" s="3" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="186" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="186" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B186" s="3" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="187" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="187" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B187" s="3" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="188" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="188" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B188" s="3" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="189" spans="2:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="189" spans="2:2" ht="30" x14ac:dyDescent="0.2">
       <c r="B189" s="3" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="190" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="190" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B190" s="3" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="191" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="191" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B191" s="3" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="192" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="192" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B192" s="3" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="193" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="193" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B193" s="3" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="194" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="194" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B194" s="3" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="195" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="195" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B195" s="3" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="196" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="196" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B196" s="3" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="197" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="197" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B197" s="3" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="198" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="198" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B198" s="3" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="199" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="199" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B199" s="3" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="200" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="200" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B200" s="3" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="201" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="201" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B201" s="3" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="202" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="202" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B202" s="3" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="203" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="203" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B203" s="3" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="204" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="204" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B204" s="3" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="205" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="205" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B205" s="3" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="206" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="206" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B206" s="3" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="207" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="207" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B207" s="3" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="208" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="208" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B208" s="3" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="209" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="209" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B209" s="3" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="210" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="210" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B210" s="3" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="211" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="211" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B211" s="3" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="212" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="212" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B212" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="213" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="213" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B213" s="3" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="214" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="214" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B214" s="3" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="215" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="215" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B215" s="3" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="216" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="216" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B216" s="3" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="217" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="217" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B217" s="3" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="218" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="218" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B218" s="3" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="219" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="219" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B219" s="3" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="220" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="220" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B220" s="3" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="221" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="221" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B221" s="3" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="222" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="222" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B222" s="3" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="223" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="223" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B223" s="3" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="224" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="224" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B224" s="3" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="225" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="225" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B225" s="3" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="226" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="226" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B226" s="3" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="227" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="227" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B227" s="3" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="228" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="228" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B228" s="3" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="229" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="229" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B229" s="3" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="230" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="230" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B230" s="3" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="231" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="231" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B231" s="3" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="232" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="232" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B232" s="3" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="233" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="233" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B233" s="3" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="234" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="234" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B234" s="3" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="235" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="235" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B235" s="3" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="236" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="236" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B236" s="3" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="237" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="237" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B237" s="3" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="238" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="238" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B238" s="3" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="239" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="239" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B239" s="3" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="240" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="240" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B240" s="3" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="241" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="241" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B241" s="3" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="242" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="242" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B242" s="3" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="243" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="243" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B243" s="3" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="244" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="244" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B244" s="3" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="245" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="245" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B245" s="3" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="246" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="246" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B246" s="3" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="247" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="247" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B247" s="3" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="248" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="248" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B248" s="3" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="249" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="2:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B249" s="3" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="250" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B250" s="5" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="251" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B251" s="5" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="252" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B252" s="5" t="s">
         <v>276</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" display="http://bioportal.bioontology.org/ontologies/ICD10CM?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FICD10CM%2FI21.3"/>
-    <hyperlink ref="B14" r:id="rId2" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10030001"/>
-    <hyperlink ref="B15" r:id="rId3" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10011108"/>
-    <hyperlink ref="B16" r:id="rId4" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10021922"/>
-    <hyperlink ref="B26" r:id="rId5" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10078240"/>
-    <hyperlink ref="B27" r:id="rId6" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10036886"/>
-    <hyperlink ref="B29" r:id="rId7" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10037705"/>
-    <hyperlink ref="B30" r:id="rId8" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10078242"/>
-    <hyperlink ref="B32" r:id="rId9" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10003674"/>
-    <hyperlink ref="B33" r:id="rId10" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10054581"/>
-    <hyperlink ref="B40" r:id="rId11" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10014387"/>
-    <hyperlink ref="B65" r:id="rId12" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10043821"/>
-    <hyperlink ref="B66" r:id="rId13" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10036359"/>
-    <hyperlink ref="B68" r:id="rId14" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10023027"/>
-    <hyperlink ref="B69" r:id="rId15" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10014515"/>
-    <hyperlink ref="B71" r:id="rId16" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10072761"/>
+    <hyperlink ref="B4" r:id="rId1" display="http://bioportal.bioontology.org/ontologies/ICD10CM?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FICD10CM%2FI21.3" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B14" r:id="rId2" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10030001" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="B15" r:id="rId3" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10011108" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="B16" r:id="rId4" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10021922" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="B26" r:id="rId5" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10078240" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="B27" r:id="rId6" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10036886" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="B29" r:id="rId7" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10037705" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="B30" r:id="rId8" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10078242" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="B32" r:id="rId9" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10003674" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="B33" r:id="rId10" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10054581" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="B40" r:id="rId11" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10014387" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
+    <hyperlink ref="B65" r:id="rId12" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10043821" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="B66" r:id="rId13" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10036359" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
+    <hyperlink ref="B68" r:id="rId14" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10023027" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
+    <hyperlink ref="B69" r:id="rId15" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10014515" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
+    <hyperlink ref="B71" r:id="rId16" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10072761" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId17"/>
@@ -3385,20 +3383,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B71"/>
   <sheetViews>
     <sheetView rightToLeft="1" topLeftCell="A40" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.19921875" customWidth="1"/>
-    <col min="2" max="2" width="36.19921875" customWidth="1"/>
+    <col min="1" max="1" width="23.1640625" customWidth="1"/>
+    <col min="2" max="2" width="36.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -3406,7 +3404,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -3414,7 +3412,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -3422,7 +3420,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -3430,7 +3428,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
@@ -3438,7 +3436,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -3446,7 +3444,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -3454,7 +3452,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -3462,7 +3460,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
@@ -3470,7 +3468,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -3478,7 +3476,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -3486,7 +3484,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
@@ -3494,7 +3492,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -3502,322 +3500,322 @@
         <v>284</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" s="7" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B15" s="7" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B16" s="7" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B17" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B18" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B20" s="8" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="8" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="22" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B22" s="8" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="23" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B23" s="7" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="24" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B24" s="7" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="25" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B25" s="8" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="26" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B26" s="7" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="27" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B27" s="8" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="28" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B28" s="8" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="29" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B29" s="7" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="30" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B30" s="8" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="31" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B31" s="7" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="32" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B32" s="8" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="33" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B33" s="7" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="34" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B34" s="7" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="35" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B35" s="8" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="36" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B36" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B37" s="7" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="38" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B38" s="8" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="39" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B39" s="8" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="40" spans="2:2" ht="30" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B40" s="7" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="41" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B41" s="8" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="42" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B42" s="7" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="43" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B43" s="7" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="44" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B44" s="7" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="45" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B45" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B46" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B47" s="8" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="48" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B48" s="8" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="49" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B49" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B50" s="7" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="51" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B51" s="8" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="52" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B52" s="8" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="53" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B53" s="8" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="54" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B54" s="8" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="55" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B55" s="8" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="56" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B56" s="8" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="57" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B57" s="2" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="58" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B58" s="2" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="59" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B59" s="2" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="60" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="62" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="63" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="64" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B64" s="2" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="65" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B65" s="3" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="66" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B66" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="68" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="69" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="70" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B71" s="2" t="s">
         <v>333</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="http://bioportal.bioontology.org/ontologies/ICD10?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FICD10%2FI05.9"/>
-    <hyperlink ref="B8" r:id="rId2" display="http://bioportal.bioontology.org/ontologies/CRISP?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FCSP%2F1393-3777"/>
-    <hyperlink ref="B10" r:id="rId3" display="http://bioportal.bioontology.org/ontologies/SNOMEDCT?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FSNOMEDCT%2F194732001"/>
-    <hyperlink ref="B26" r:id="rId4" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10026985"/>
+    <hyperlink ref="B2" r:id="rId1" display="http://bioportal.bioontology.org/ontologies/ICD10?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FICD10%2FI05.9" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="B8" r:id="rId2" display="http://bioportal.bioontology.org/ontologies/CRISP?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FCSP%2F1393-3777" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="B10" r:id="rId3" display="http://bioportal.bioontology.org/ontologies/SNOMEDCT?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FSNOMEDCT%2F194732001" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="B26" r:id="rId4" display="http://bioportal.bioontology.org/ontologies/MEDDRA?p=classes&amp;conceptid=http%3A%2F%2Fpurl.bioontology.org%2Fontology%2FMEDDRA%2F10026985" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B322"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="A304" workbookViewId="0">
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A310" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B323"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.59765625" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
     <col min="2" max="2" width="46" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -3825,7 +3823,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -3833,7 +3831,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -3841,7 +3839,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -3849,7 +3847,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
@@ -3857,7 +3855,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -3865,7 +3863,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -3873,7 +3871,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -3881,7 +3879,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
@@ -3889,7 +3887,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -3897,7 +3895,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -3905,7 +3903,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
@@ -3913,7 +3911,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -3921,7 +3919,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -3929,7 +3927,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -3937,7 +3935,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -3945,7 +3943,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -3953,1527 +3951,1527 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B20" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B21" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B23" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B24" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B26" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B27" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B28" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B29" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B30" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B31" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B32" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B36" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B37" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="38" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B38" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B39" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B40" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B41" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B42" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B43" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="44" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B44" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="45" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B45" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="46" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B46" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B47" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="48" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B48" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="49" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B49" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="50" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B50" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="51" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B51" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="52" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B52" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="53" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B53" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="54" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B54" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="55" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B55" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="56" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B56" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="57" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B57" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="58" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B58" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="59" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B59" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="60" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B60" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="61" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B61" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="62" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B62" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="63" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B63" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="64" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B64" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="65" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B65" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="66" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B66" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="67" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="68" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B68" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="69" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B69" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="70" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B70" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="71" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B71" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="72" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B72" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="73" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B73" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="74" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B74" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="75" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B75" s="6" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="76" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="77" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B77" s="4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="78" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B78" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="79" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B79" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="80" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B80" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="81" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B81" s="5" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="82" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B82" s="5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="83" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B83" s="5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="84" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B84" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="85" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B85" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="86" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B86" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="87" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B87" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="88" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B88" s="5" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="89" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B89" s="4" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="90" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B90" s="5" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="91" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B91" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="92" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B92" s="4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="93" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B93" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="94" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B94" s="5" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="95" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B95" s="4" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="96" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B96" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B97" s="4" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="98" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B98" s="5" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="99" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B99" s="5" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="100" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B100" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="101" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B101" s="4" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="102" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B102" s="3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="103" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B103" s="4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="104" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B104" s="4" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="105" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B105" s="5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="106" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B106" s="4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="107" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B107" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="108" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B108" s="5" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="109" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B109" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B110" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B111" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="112" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B112" s="4" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="113" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B113" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="114" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B114" s="4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="115" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B115" s="3" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="116" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B116" s="3" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="117" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B117" s="4" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="118" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B118" s="4" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="119" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B119" s="5" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="120" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B120" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B121" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B122" s="4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="123" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B123" s="4" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="124" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B124" s="5" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="125" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B125" s="5" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="126" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B126" s="5" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="127" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B127" s="5" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="128" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B128" s="4" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="129" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B129" s="5" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="130" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B130" s="4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="131" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B131" s="4" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="132" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B132" s="3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="133" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="133" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B133" s="3" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="134" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="134" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B134" s="3" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="135" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B135" s="3" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="136" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B136" s="3" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="137" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B137" s="3" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="138" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B138" s="3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="139" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B139" s="3" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="140" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B140" s="3" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="141" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B141" s="3" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="142" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B142" s="3" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="143" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B143" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="144" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="144" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B144" s="3" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="145" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="145" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B145" s="4" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="146" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B146" s="4" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="147" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B147" s="5" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="148" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B148" s="5" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="149" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B149" s="4" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="150" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B150" s="2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="151" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B151" s="3" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="152" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B152" s="3" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="153" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B153" s="3" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="154" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B154" s="3" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="155" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="155" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B155" s="3" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="156" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="156" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B156" s="3" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="157" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="157" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B157" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="158" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B158" s="3" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="159" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="159" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B159" s="3" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="160" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="160" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B160" s="3" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="161" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="161" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B161" s="3" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="162" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="162" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B162" s="3" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="163" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="163" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B163" s="3" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="164" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="164" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B164" s="3" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="165" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="165" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B165" s="3" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="166" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="166" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B166" s="3" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="167" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="167" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B167" s="3" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="168" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="168" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B168" s="3" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="169" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="169" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B169" s="3" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="170" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="170" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B170" s="3" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="171" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="171" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B171" s="3" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="172" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="172" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B172" s="3" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="173" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="173" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B173" s="3" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="174" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="174" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B174" s="3" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="175" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="175" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B175" s="3" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="176" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="176" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B176" s="3" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="177" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="177" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B177" s="3" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="178" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="178" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B178" s="3" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="179" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="179" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B179" s="3" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="180" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="180" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B180" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="181" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="181" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B181" s="3" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="182" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="182" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B182" s="3" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="183" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="183" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B183" s="3" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="184" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="184" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B184" s="3" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="185" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="185" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B185" s="3" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="186" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="186" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B186" s="3" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="187" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="187" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B187" s="3" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="188" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="188" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B188" s="3" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="189" spans="2:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="189" spans="2:2" ht="30" x14ac:dyDescent="0.2">
       <c r="B189" s="3" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="190" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="190" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B190" s="3" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="191" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="191" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B191" s="3" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="192" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="192" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B192" s="3" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="193" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="193" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B193" s="3" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="194" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="194" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B194" s="3" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="195" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="195" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B195" s="3" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="196" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="196" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B196" s="3" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="197" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="197" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B197" s="3" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="198" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="198" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B198" s="3" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="199" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="199" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B199" s="3" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="200" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="200" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B200" s="3" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="201" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="201" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B201" s="3" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="202" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="202" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B202" s="3" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="203" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="203" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B203" s="3" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="204" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="204" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B204" s="3" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="205" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="205" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B205" s="3" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="206" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="206" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B206" s="3" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="207" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="207" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B207" s="3" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="208" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="208" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B208" s="3" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="209" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="209" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B209" s="3" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="210" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="210" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B210" s="3" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="211" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="211" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B211" s="3" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="212" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="212" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B212" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="213" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="213" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B213" s="3" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="214" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="214" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B214" s="3" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="215" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="215" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B215" s="3" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="216" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="216" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B216" s="3" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="217" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="217" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B217" s="3" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="218" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="218" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B218" s="3" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="219" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="219" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B219" s="3" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="220" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="220" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B220" s="3" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="221" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="221" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B221" s="3" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="222" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="222" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B222" s="3" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="223" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="223" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B223" s="3" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="224" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="224" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B224" s="3" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="225" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="225" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B225" s="3" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="226" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="226" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B226" s="3" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="227" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="227" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B227" s="3" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="228" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="228" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B228" s="3" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="229" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="229" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B229" s="3" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="230" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="230" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B230" s="3" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="231" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="231" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B231" s="3" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="232" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="232" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B232" s="3" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="233" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="233" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B233" s="3" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="234" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="234" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B234" s="3" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="235" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="235" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B235" s="3" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="236" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="236" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B236" s="3" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="237" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="237" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B237" s="3" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="238" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="238" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B238" s="3" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="239" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="239" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B239" s="3" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="240" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="240" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B240" s="3" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="241" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="241" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B241" s="3" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="242" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="242" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B242" s="3" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="243" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="243" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B243" s="3" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="244" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="244" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B244" s="3" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="245" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="245" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B245" s="3" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="246" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="246" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B246" s="3" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="247" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="247" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B247" s="3" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="248" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="248" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B248" s="3" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="249" spans="2:2" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="2:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B249" s="3" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="250" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B250" s="5" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="251" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B251" s="5" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="252" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="2:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B252" s="5" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="253" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="253" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B253" s="3" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="254" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="254" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B254" s="3" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="255" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="255" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B255" s="3" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="256" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="256" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B256" s="3" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="257" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="257" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B257" s="3" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="258" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="258" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B258" s="3" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="259" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="259" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B259" s="4" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="260" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="260" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B260" s="4" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="261" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="261" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B261" s="4" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="262" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="262" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B262" s="2" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="263" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="263" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B263" s="3" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="264" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="264" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B264" s="7" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="265" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="265" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B265" s="7" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="266" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="266" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B266" s="7" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="267" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="267" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B267" s="7" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="268" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="268" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B268" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="269" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="269" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B269" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="270" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="270" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B270" s="7" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="271" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="271" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B271" s="8" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="272" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="272" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B272" s="8" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="273" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="273" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B273" s="8" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="274" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="274" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B274" s="7" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="275" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="275" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B275" s="7" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="276" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="276" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B276" s="8" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="277" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="277" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B277" s="7" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="278" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="278" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B278" s="8" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="279" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="279" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B279" s="8" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="280" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="280" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B280" s="7" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="281" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="281" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B281" s="8" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="282" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="282" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B282" s="7" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="283" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="283" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B283" s="8" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="284" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="284" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B284" s="7" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="285" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="285" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B285" s="7" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="286" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="286" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B286" s="8" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="287" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="287" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B287" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="288" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="288" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B288" s="7" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="289" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="289" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B289" s="8" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="290" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="290" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B290" s="8" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="291" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="291" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B291" s="7" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="292" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="292" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B292" s="8" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="293" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="293" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B293" s="7" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="294" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="294" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B294" s="7" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="295" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="295" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B295" s="7" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="296" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="296" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B296" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="297" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="297" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B297" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="298" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="298" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B298" s="8" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="299" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="299" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B299" s="8" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="300" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="300" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B300" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="301" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="301" spans="2:2" ht="17" x14ac:dyDescent="0.2">
       <c r="B301" s="7" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="302" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="302" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B302" s="8" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="303" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="303" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B303" s="8" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="304" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="304" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B304" s="8" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="305" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="305" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B305" s="8" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="306" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="306" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B306" s="8" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="307" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="307" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B307" s="8" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="308" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="308" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B308" s="2" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="309" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="309" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B309" s="2" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="310" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="310" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B310" s="2" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="311" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="311" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B311" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="312" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="312" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B312" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="313" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="313" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B313" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="314" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="314" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B314" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="315" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="315" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B315" s="2" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="316" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="316" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B316" s="3" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="317" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="317" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B317" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="318" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="318" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B318" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="319" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="319" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B319" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="320" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="320" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B320" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="321" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="321" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B321" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="322" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="322" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B322" s="2" t="s">
         <v>333</v>
       </c>

</xml_diff>